<commit_message>
Add check for officer when applyinh
</commit_message>
<xml_diff>
--- a/sc2002/src/main/resources/OfficerList.xlsx
+++ b/sc2002/src/main/resources/OfficerList.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew Chan\Documents\GitHub\SC2002\sc2002\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\NTUWorkspace\Y1 Y2\Object Oriented Design &amp; Programming\project\sc2002\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52BDCE8B-9982-45E4-BFCC-7F67D0478EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1217A02C-0F7F-4D72-AE12-75D13688BDCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6675" yWindow="3735" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40305" yWindow="8910" windowWidth="19200" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -384,12 +384,12 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -406,7 +406,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -423,7 +423,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -440,7 +440,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -448,7 +448,7 @@
         <v>12</v>
       </c>
       <c r="C4">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>

</xml_diff>